<commit_message>
fix loi import excel
</commit_message>
<xml_diff>
--- a/Computer_Shop/src/excel/list sp.xlsx
+++ b/Computer_Shop/src/excel/list sp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trong Phu\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trong Phu\Documents\GitHub\ComputerShop\Computer_Shop\src\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267B01DB-4499-4C66-95EC-8BED97C09EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521A954A-B209-4D6D-993D-BBA7C7E00B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99D031B9-0158-4D4E-8374-12C5AA17CE8F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="105">
   <si>
     <t>AC0006</t>
   </si>
@@ -304,6 +304,42 @@
   </si>
   <si>
     <t>13.6", Liquid Retina (2560 x 1664)</t>
+  </si>
+  <si>
+    <t>Mã sản phẩm</t>
+  </si>
+  <si>
+    <t>Tên sản phẩm</t>
+  </si>
+  <si>
+    <t>Hình ảnh</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>ROM</t>
+  </si>
+  <si>
+    <t>Card đồ hoạ</t>
+  </si>
+  <si>
+    <t>Màn hình</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Hãng</t>
+  </si>
+  <si>
+    <t>Giá</t>
+  </si>
+  <si>
+    <t>Tình trạng</t>
   </si>
 </sst>
 </file>
@@ -663,14 +699,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0D99BD-6BCE-468D-8558-E4196A447449}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="24.5546875" customWidth="1"/>
     <col min="4" max="4" width="21.5546875" customWidth="1"/>
@@ -679,79 +716,80 @@
     <col min="7" max="7" width="22.5546875" customWidth="1"/>
     <col min="8" max="8" width="36" customWidth="1"/>
     <col min="9" max="9" width="19.21875" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1">
-        <v>17990000</v>
-      </c>
-      <c r="L1">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K2">
-        <v>18490000</v>
+        <v>17990000</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -759,19 +797,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -780,16 +818,16 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
         <v>4</v>
       </c>
       <c r="K3">
-        <v>13690000</v>
+        <v>18490000</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -797,16 +835,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -814,20 +852,20 @@
       <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
         <v>4</v>
       </c>
       <c r="K4">
-        <v>20990000</v>
+        <v>13690000</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -835,37 +873,37 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
-        <v>36</v>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="K5">
-        <v>13490000</v>
+        <v>20990000</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -873,37 +911,37 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
         <v>39</v>
       </c>
       <c r="K6">
-        <v>20990000</v>
+        <v>13490000</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -911,19 +949,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
@@ -932,16 +970,16 @@
         <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="J7" t="s">
         <v>39</v>
       </c>
       <c r="K7">
-        <v>19790000</v>
+        <v>20990000</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -949,37 +987,37 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
+      </c>
+      <c r="I8" t="s">
+        <v>51</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="K8">
-        <v>10990000</v>
+        <v>19790000</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -987,22 +1025,22 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
         <v>57</v>
@@ -1017,7 +1055,7 @@
         <v>60</v>
       </c>
       <c r="K9">
-        <v>16490000</v>
+        <v>10990000</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1025,25 +1063,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>58</v>
@@ -1055,7 +1093,7 @@
         <v>60</v>
       </c>
       <c r="K10">
-        <v>18390000</v>
+        <v>16490000</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -1063,13 +1101,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
         <v>64</v>
@@ -1081,19 +1119,19 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="J11" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="K11">
-        <v>13990000</v>
+        <v>18390000</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1101,16 +1139,16 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
@@ -1119,19 +1157,19 @@
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
         <v>73</v>
       </c>
       <c r="K12">
-        <v>17190000</v>
+        <v>13990000</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1139,37 +1177,37 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>83</v>
+        <v>57</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J13" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="K13">
-        <v>18990000</v>
+        <v>17190000</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -1177,16 +1215,16 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
         <v>82</v>
@@ -1195,10 +1233,10 @@
         <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>84</v>
@@ -1207,9 +1245,47 @@
         <v>85</v>
       </c>
       <c r="K14">
+        <v>18990000</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J15" t="s">
+        <v>85</v>
+      </c>
+      <c r="K15">
         <v>26990000</v>
       </c>
-      <c r="L14">
+      <c r="L15">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
them validate data khi import excel (chua hoan thien lam)
</commit_message>
<xml_diff>
--- a/Computer_Shop/src/excel/list sp.xlsx
+++ b/Computer_Shop/src/excel/list sp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trong Phu\Documents\GitHub\ComputerShop\Computer_Shop\src\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521A954A-B209-4D6D-993D-BBA7C7E00B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7918A03A-AC78-4BC4-AD7F-09CF7DFA7998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99D031B9-0158-4D4E-8374-12C5AA17CE8F}"/>
   </bookViews>
@@ -702,7 +702,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
chinh sua 1 ti phan them san pham
</commit_message>
<xml_diff>
--- a/Computer_Shop/src/excel/list sp.xlsx
+++ b/Computer_Shop/src/excel/list sp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trong Phu\Documents\GitHub\ComputerShop\Computer_Shop\src\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7918A03A-AC78-4BC4-AD7F-09CF7DFA7998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0586162A-2139-4A06-A358-D32D5341CB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99D031B9-0158-4D4E-8374-12C5AA17CE8F}"/>
   </bookViews>
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0D99BD-6BCE-468D-8558-E4196A447449}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fix loi import anh
</commit_message>
<xml_diff>
--- a/Computer_Shop/src/excel/list sp.xlsx
+++ b/Computer_Shop/src/excel/list sp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trong Phu\Documents\GitHub\ComputerShop\Computer_Shop\src\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7918A03A-AC78-4BC4-AD7F-09CF7DFA7998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6704ABF-10F3-4D19-AA06-F9F972FA5F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99D031B9-0158-4D4E-8374-12C5AA17CE8F}"/>
   </bookViews>
@@ -282,9 +282,6 @@
     <t>18 giờ</t>
   </si>
   <si>
-    <t>Macbook</t>
-  </si>
-  <si>
     <t>Laptop Apple MacBook Air 13 inch M2 2022</t>
   </si>
   <si>
@@ -340,6 +337,9 @@
   </si>
   <si>
     <t>Tình trạng</t>
+  </si>
+  <si>
+    <t>Apple</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,40 +721,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>95</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>101</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>102</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>103</v>
-      </c>
-      <c r="L1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1233,7 +1233,7 @@
         <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>83</v>
@@ -1242,7 +1242,7 @@
         <v>84</v>
       </c>
       <c r="J14" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="K14">
         <v>18990000</v>
@@ -1253,16 +1253,16 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
         <v>87</v>
       </c>
-      <c r="B15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>88</v>
-      </c>
-      <c r="D15" t="s">
-        <v>89</v>
       </c>
       <c r="E15" t="s">
         <v>82</v>
@@ -1271,16 +1271,16 @@
         <v>56</v>
       </c>
       <c r="G15" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>84</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="K15">
         <v>26990000</v>
@@ -1291,5 +1291,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>